<commit_message>
windowmanager new resize bindings and keeping order of spaces on macos
</commit_message>
<xml_diff>
--- a/windowmanager/shortcuts.xlsx
+++ b/windowmanager/shortcuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruud.wijtvliet/.dotfiles/windowmanager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875EC223-B507-6141-94A2-C9C96E2F1B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E3B34-9F1D-AF4B-AFF1-6367D7101687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33160" yWindow="1100" windowWidth="26800" windowHeight="31940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30180" yWindow="700" windowWidth="29780" windowHeight="32340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shortcuts" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="154">
   <si>
     <t>ENTER</t>
   </si>
@@ -361,9 +361,6 @@
     <t>→</t>
   </si>
   <si>
-    <t>up/left/down/right</t>
-  </si>
-  <si>
     <t>window to</t>
   </si>
   <si>
@@ -457,9 +454,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>float/tiled</t>
   </si>
   <si>
@@ -496,12 +490,6 @@
     <t>f = firefox,</t>
   </si>
   <si>
-    <t>set layout</t>
-  </si>
-  <si>
-    <t>to split</t>
-  </si>
-  <si>
     <t>vertical</t>
   </si>
   <si>
@@ -593,6 +581,21 @@
   </si>
   <si>
     <t>character in def)</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>sizes</t>
+  </si>
+  <si>
+    <t>set to split</t>
+  </si>
+  <si>
+    <t>(= insert below)</t>
+  </si>
+  <si>
+    <t>(= insert on right)</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1108,6 +1111,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1120,12 +1141,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1144,27 +1159,14 @@
     <xf numFmtId="8" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -1491,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:U76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1524,40 +1526,40 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E5" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="J5" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="K5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="L5" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="77" t="s">
+      <c r="M5" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="N5" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="O5" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="P5" s="50" t="s">
         <v>136</v>
-      </c>
-      <c r="M5" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="N5" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="O5" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="P5" s="50" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
@@ -1567,17 +1569,17 @@
       <c r="E6" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="94" t="s">
+      <c r="F6" s="82" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1590,41 +1592,41 @@
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="78"/>
       <c r="E7" s="70" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" s="95" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="F7" s="83" t="s">
+        <v>122</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H7" s="81" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
       <c r="P7" s="81"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="78"/>
       <c r="E8" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="96" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="F8" s="84" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="15"/>
@@ -1638,19 +1640,19 @@
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="78"/>
       <c r="E9" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J9" s="75"/>
       <c r="K9" s="75"/>
@@ -1663,19 +1665,19 @@
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="78"/>
       <c r="E10" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" s="79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J10" s="75"/>
       <c r="K10" s="75"/>
@@ -1715,7 +1717,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
+      <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="4"/>
@@ -1723,25 +1725,25 @@
         <v>1</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D14" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="87"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="100"/>
       <c r="O14" s="12" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1760,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D15" s="37" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1769,7 +1771,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
+      <c r="N15" s="17"/>
       <c r="O15" s="17" t="s">
         <v>20</v>
       </c>
@@ -1786,26 +1788,26 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D16" s="45"/>
-      <c r="E16" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="90"/>
+      <c r="E16" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="101"/>
       <c r="O16" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="T16" s="2">
@@ -1817,26 +1819,26 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D17" s="45"/>
-      <c r="E17" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="89"/>
-      <c r="N17" s="90"/>
+      <c r="E17" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="101"/>
       <c r="O17" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="T17" s="2">
@@ -1851,40 +1853,40 @@
         <v>10</v>
       </c>
       <c r="E18" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="52" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="I18" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="52" t="s">
+      <c r="K18" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="L18" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="52" t="s">
+      <c r="M18" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="N18" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N18" s="53" t="s">
+      <c r="O18" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="O18" s="60" t="s">
+      <c r="P18" s="60" t="s">
         <v>91</v>
-      </c>
-      <c r="P18" s="60" t="s">
-        <v>92</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="T18" s="2">
@@ -1907,7 +1909,9 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="8"/>
+      <c r="N19" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="O19" s="7"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="4"/>
@@ -1920,20 +1924,22 @@
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D20" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="84"/>
+        <v>137</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="O20" s="22" t="s">
         <v>21</v>
       </c>
@@ -1950,7 +1956,7 @@
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D21" s="37" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
@@ -1961,7 +1967,9 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="16"/>
+      <c r="N21" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="O21" s="15" t="s">
         <v>22</v>
       </c>
@@ -1978,45 +1986,49 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D22" s="45"/>
-      <c r="E22" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="89"/>
-      <c r="L22" s="89"/>
-      <c r="M22" s="89"/>
-      <c r="N22" s="90"/>
+      <c r="E22" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="93"/>
+      <c r="L22" s="93"/>
+      <c r="M22" s="93"/>
+      <c r="N22" s="41" t="s">
+        <v>105</v>
+      </c>
       <c r="O22" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D23" s="45"/>
-      <c r="E23" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="89"/>
-      <c r="M23" s="89"/>
-      <c r="N23" s="90"/>
+      <c r="E23" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="93"/>
+      <c r="K23" s="93"/>
+      <c r="L23" s="93"/>
+      <c r="M23" s="93"/>
+      <c r="N23" s="41" t="s">
+        <v>109</v>
+      </c>
       <c r="O23" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q23" s="4"/>
     </row>
@@ -2041,13 +2053,13 @@
         <v>12</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="98" t="s">
+      <c r="E26" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="98" t="s">
+      <c r="F26" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="98" t="s">
+      <c r="G26" s="85" t="s">
         <v>28</v>
       </c>
       <c r="H26" s="24"/>
@@ -2067,27 +2079,27 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D27" s="4"/>
-      <c r="E27" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="G27" s="99" t="s">
-        <v>151</v>
+      <c r="E27" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="86" t="s">
+        <v>147</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O27" s="26"/>
       <c r="P27" s="10"/>
@@ -2095,27 +2107,27 @@
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
-      <c r="E28" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="F28" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="G28" s="100" t="s">
-        <v>152</v>
+      <c r="E28" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="87" t="s">
+        <v>148</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O28" s="18"/>
       <c r="P28" s="13"/>
@@ -2130,12 +2142,12 @@
       <c r="I29" s="41"/>
       <c r="J29" s="41"/>
       <c r="K29" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
       <c r="N29" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="41"/>
@@ -2150,12 +2162,12 @@
       <c r="I30" s="41"/>
       <c r="J30" s="41"/>
       <c r="K30" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
       <c r="N30" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="41"/>
@@ -2207,17 +2219,17 @@
         <v>11</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="85" t="s">
         <v>28</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I32" s="38"/>
       <c r="J32" s="6"/>
@@ -2231,29 +2243,29 @@
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D33" s="4"/>
-      <c r="E33" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="F33" s="99" t="s">
-        <v>151</v>
-      </c>
-      <c r="G33" s="99" t="s">
-        <v>151</v>
+      <c r="E33" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="86" t="s">
+        <v>147</v>
       </c>
       <c r="H33" s="43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I33" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J33" s="21"/>
       <c r="K33" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="L33" s="82"/>
-      <c r="M33" s="84"/>
+        <v>98</v>
+      </c>
+      <c r="L33" s="88"/>
+      <c r="M33" s="90"/>
       <c r="N33" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O33" s="26"/>
       <c r="P33" s="10"/>
@@ -2261,27 +2273,27 @@
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D34" s="4"/>
-      <c r="E34" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="100" t="s">
-        <v>152</v>
+      <c r="E34" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="87" t="s">
+        <v>148</v>
       </c>
       <c r="H34" s="44"/>
       <c r="I34" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L34" s="14"/>
       <c r="M34" s="16"/>
       <c r="N34" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O34" s="18"/>
       <c r="P34" s="13"/>
@@ -2293,17 +2305,17 @@
       <c r="F35" s="41"/>
       <c r="G35" s="41"/>
       <c r="H35" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I35" s="46"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
       <c r="N35" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O35" s="41"/>
       <c r="P35" s="41"/>
@@ -2318,12 +2330,12 @@
       <c r="I36" s="46"/>
       <c r="J36" s="41"/>
       <c r="K36" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
       <c r="N36" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
@@ -2385,21 +2397,21 @@
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D40" s="4"/>
       <c r="E40" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="27"/>
       <c r="J40" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="K40" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="K40" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="83"/>
-      <c r="M40" s="83"/>
-      <c r="N40" s="84"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="90"/>
       <c r="O40" s="10" t="s">
         <v>1</v>
       </c>
@@ -2409,14 +2421,14 @@
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D41" s="4"/>
       <c r="E41" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
       <c r="I41" s="20"/>
       <c r="J41" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K41" s="14"/>
       <c r="L41" s="15"/>
@@ -2429,19 +2441,19 @@
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D42" s="4"/>
       <c r="E42" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="41"/>
-      <c r="K42" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="L42" s="89"/>
-      <c r="M42" s="89"/>
-      <c r="N42" s="90"/>
+      <c r="K42" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="94"/>
       <c r="O42" s="41"/>
       <c r="P42" s="46"/>
       <c r="Q42" s="4"/>
@@ -2449,21 +2461,21 @@
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D43" s="4"/>
       <c r="E43" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>
       <c r="I43" s="41"/>
       <c r="J43" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="K43" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="L43" s="89"/>
-      <c r="M43" s="89"/>
-      <c r="N43" s="90"/>
+        <v>105</v>
+      </c>
+      <c r="K43" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="94"/>
       <c r="O43" s="41"/>
       <c r="P43" s="46"/>
       <c r="Q43" s="4"/>
@@ -2532,21 +2544,21 @@
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
       <c r="E46" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="27"/>
       <c r="J46" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K46" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="K46" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="92"/>
-      <c r="M46" s="92"/>
-      <c r="N46" s="93"/>
+      <c r="L46" s="96"/>
+      <c r="M46" s="96"/>
+      <c r="N46" s="97"/>
       <c r="O46" s="10"/>
       <c r="P46" s="32" t="s">
         <v>33</v>
@@ -2556,14 +2568,14 @@
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D47" s="4"/>
       <c r="E47" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
       <c r="I47" s="20"/>
       <c r="J47" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K47" s="14"/>
       <c r="L47" s="15"/>
@@ -2576,46 +2588,46 @@
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
       <c r="E48" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="L48" s="89"/>
-      <c r="M48" s="89"/>
-      <c r="N48" s="90"/>
+      <c r="K48" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="94"/>
       <c r="O48" s="41"/>
       <c r="P48" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q48" s="4"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D49" s="4"/>
       <c r="E49" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
       <c r="H49" s="41"/>
       <c r="I49" s="41"/>
       <c r="J49" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="K49" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="L49" s="89"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="90"/>
+        <v>105</v>
+      </c>
+      <c r="K49" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="93"/>
+      <c r="M49" s="93"/>
+      <c r="N49" s="94"/>
       <c r="O49" s="41"/>
       <c r="P49" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q49" s="4"/>
     </row>
@@ -2652,7 +2664,7 @@
         <v>12</v>
       </c>
       <c r="D52" s="4"/>
-      <c r="E52" s="98" t="s">
+      <c r="E52" s="85" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="35" t="s">
@@ -2667,10 +2679,10 @@
       <c r="K52" s="9"/>
       <c r="L52" s="5"/>
       <c r="M52" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="N52" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="N52" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="O52" s="4"/>
       <c r="R52" s="9"/>
@@ -2679,8 +2691,8 @@
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D53" s="4"/>
-      <c r="E53" s="99" t="s">
-        <v>151</v>
+      <c r="E53" s="86" t="s">
+        <v>147</v>
       </c>
       <c r="F53" s="36" t="s">
         <v>67</v>
@@ -2689,30 +2701,32 @@
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K53" s="12" t="s">
         <v>24</v>
       </c>
       <c r="L53" s="10"/>
       <c r="M53" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O53" s="4"/>
       <c r="Q53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R53" s="12"/>
-      <c r="S53" s="12"/>
+      <c r="S53" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="T53" s="12"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D54" s="4"/>
-      <c r="E54" s="100" t="s">
-        <v>152</v>
+      <c r="E54" s="87" t="s">
+        <v>148</v>
       </c>
       <c r="F54" s="37" t="s">
         <v>68</v>
@@ -2721,22 +2735,22 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
       <c r="J54" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K54" s="17" t="s">
         <v>25</v>
       </c>
       <c r="L54" s="13"/>
       <c r="M54" s="17" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O54" s="4"/>
       <c r="R54" s="12"/>
       <c r="S54" s="12" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="T54" s="12"/>
     </row>
@@ -2748,20 +2762,20 @@
       <c r="H55" s="41"/>
       <c r="I55" s="41"/>
       <c r="J55" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K55" s="41"/>
       <c r="L55" s="41"/>
       <c r="M55" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N55" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O55" s="4"/>
       <c r="R55" s="41"/>
       <c r="S55" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T55" s="41"/>
     </row>
@@ -2776,15 +2790,15 @@
       <c r="K56" s="41"/>
       <c r="L56" s="41"/>
       <c r="M56" s="41" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="N56" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O56" s="4"/>
       <c r="R56" s="41"/>
       <c r="S56" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T56" s="41"/>
     </row>
@@ -2836,7 +2850,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="4"/>
-      <c r="E58" s="98" t="s">
+      <c r="E58" s="85" t="s">
         <v>28</v>
       </c>
       <c r="F58" s="35" t="s">
@@ -2855,30 +2869,28 @@
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="9" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q58" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R58" s="6"/>
-      <c r="S58" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="S58" s="7"/>
       <c r="T58" s="8"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
-      <c r="E59" s="99" t="s">
-        <v>151</v>
+      <c r="E59" s="86" t="s">
+        <v>147</v>
       </c>
       <c r="F59" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H59" s="12"/>
       <c r="I59" s="10"/>
@@ -2892,34 +2904,38 @@
         <v>17</v>
       </c>
       <c r="M59" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="R59" s="82" t="s">
-        <v>75</v>
-      </c>
-      <c r="S59" s="83"/>
-      <c r="T59" s="84"/>
+        <v>115</v>
+      </c>
+      <c r="R59" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="S59" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="T59" s="81" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D60" s="4"/>
-      <c r="E60" s="100" t="s">
-        <v>152</v>
+      <c r="E60" s="87" t="s">
+        <v>148</v>
       </c>
       <c r="F60" s="37" t="s">
         <v>68</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H60" s="17" t="s">
         <v>1</v>
       </c>
       <c r="I60" s="13"/>
       <c r="J60" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K60" s="17" t="s">
         <v>66</v>
@@ -2928,74 +2944,80 @@
         <v>25</v>
       </c>
       <c r="M60" s="17" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="N60" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="R60" s="14"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="16"/>
+        <v>113</v>
+      </c>
+      <c r="R60" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="S60" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T60" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D61" s="4"/>
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
       <c r="G61" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H61" s="41"/>
       <c r="I61" s="41"/>
       <c r="J61" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K61" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L61" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M61" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N61" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="R61" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="S61" s="89"/>
-      <c r="T61" s="90"/>
+        <v>105</v>
+      </c>
+      <c r="R61" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="S61" s="93"/>
+      <c r="T61" s="94"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D62" s="4"/>
       <c r="E62" s="41"/>
       <c r="F62" s="41"/>
       <c r="G62" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H62" s="41"/>
       <c r="I62" s="41"/>
       <c r="J62" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K62" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L62" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M62" s="41" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="N62" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="R62" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="S62" s="89"/>
-      <c r="T62" s="90"/>
+        <v>109</v>
+      </c>
+      <c r="R62" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="S62" s="93"/>
+      <c r="T62" s="94"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D63" s="4"/>
@@ -3022,7 +3044,7 @@
     <row r="64" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3035,7 +3057,7 @@
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
       <c r="R64" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.2">
@@ -3050,7 +3072,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="R65" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.2">
@@ -3072,7 +3094,7 @@
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
       <c r="R66" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.2">
@@ -3182,7 +3204,7 @@
         <v>29</v>
       </c>
       <c r="J73" s="73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -3225,23 +3247,22 @@
       <c r="J76" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="R61:T61"/>
     <mergeCell ref="R62:T62"/>
-    <mergeCell ref="R59:T59"/>
     <mergeCell ref="K46:N46"/>
     <mergeCell ref="K40:N40"/>
     <mergeCell ref="K42:N42"/>
     <mergeCell ref="K43:N43"/>
     <mergeCell ref="K48:N48"/>
     <mergeCell ref="K49:N49"/>
-    <mergeCell ref="E20:N20"/>
-    <mergeCell ref="E14:N14"/>
     <mergeCell ref="L33:M33"/>
-    <mergeCell ref="E16:N16"/>
-    <mergeCell ref="E17:N17"/>
-    <mergeCell ref="E22:N22"/>
-    <mergeCell ref="E23:N23"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E22:M22"/>
+    <mergeCell ref="E23:M23"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:P11">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="~?">
@@ -3254,7 +3275,7 @@
       <formula>NOT(ISERROR(SEARCH("yes",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:P17 E22:P23 E29:Q30 E35:Q36 E42:P43 E48:P49 E55:N56 R55:T56 E61:N62 R61:R62">
+  <conditionalFormatting sqref="N22:P23 E29:Q30 E35:Q36 E42:P43 E48:P49 E55:N56 R55:T56 E61:N62 R61:R62 E16:E17 N16:P17 E22:E23">
     <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="~?">
       <formula>NOT(ISERROR(SEARCH("~?",E16)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated windowmanager because it broke again after macos update
</commit_message>
<xml_diff>
--- a/windowmanager/shortcuts.xlsx
+++ b/windowmanager/shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruud.wijtvliet/.dotfiles/windowmanager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA50186-BE6B-544D-A61E-3532432D961A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35396B44-CD2D-2749-8B32-726C89887497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33160" yWindow="700" windowWidth="26800" windowHeight="32400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="960" windowWidth="33020" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shortcuts" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
   <si>
     <t>ENTER</t>
   </si>
@@ -452,9 +452,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>float/tiled</t>
   </si>
   <si>
     <t>parent</t>
@@ -1131,6 +1128,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1147,21 +1159,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1490,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:U76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,40 +1520,40 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E5" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="G5" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="H5" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="I5" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="77" t="s">
+      <c r="J5" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="K5" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="L5" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="M5" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="N5" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="O5" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="P5" s="50" t="s">
         <v>135</v>
-      </c>
-      <c r="P5" s="50" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
@@ -1570,13 +1567,13 @@
         <v>30</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="72" t="s">
         <v>144</v>
-      </c>
-      <c r="I6" s="72" t="s">
-        <v>145</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1589,19 +1586,19 @@
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="78"/>
       <c r="E7" s="70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H7" s="81" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="73" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -1614,16 +1611,16 @@
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="78"/>
       <c r="E8" s="71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I8" s="74"/>
       <c r="J8" s="15"/>
@@ -1727,19 +1724,19 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D14" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="99" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
       <c r="N14" s="88"/>
       <c r="O14" s="12" t="s">
         <v>21</v>
@@ -1757,7 +1754,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D15" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1785,20 +1782,20 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="45"/>
-      <c r="E16" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="91"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="91"/>
+      <c r="E16" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="96"/>
       <c r="N16" s="89"/>
       <c r="O16" s="13" t="s">
         <v>105</v>
@@ -1816,26 +1813,26 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" s="45"/>
-      <c r="E17" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
+      <c r="E17" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
       <c r="N17" s="89"/>
       <c r="O17" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="T17" s="2">
@@ -1907,7 +1904,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O19" s="7"/>
       <c r="P19" s="9"/>
@@ -1921,19 +1918,19 @@
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D20" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="E20" s="96" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="97"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="97"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
       <c r="N20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1953,7 +1950,7 @@
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D21" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
@@ -1965,7 +1962,7 @@
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
       <c r="N21" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O21" s="15" t="s">
         <v>22</v>
@@ -1983,17 +1980,17 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D22" s="45"/>
-      <c r="E22" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
+      <c r="E22" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
       <c r="N22" s="41" t="s">
         <v>105</v>
       </c>
@@ -2007,25 +2004,25 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D23" s="45"/>
-      <c r="E23" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
+      <c r="E23" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
       <c r="N23" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q23" s="4"/>
     </row>
@@ -2077,13 +2074,13 @@
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D27" s="4"/>
       <c r="E27" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F27" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G27" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="43" t="s">
@@ -2105,13 +2102,13 @@
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F28" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G28" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="44" t="s">
@@ -2226,7 +2223,7 @@
         <v>28</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I32" s="38"/>
       <c r="J32" s="6"/>
@@ -2241,16 +2238,16 @@
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D33" s="4"/>
       <c r="E33" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F33" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G33" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H33" s="43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I33" s="39" t="s">
         <v>93</v>
@@ -2259,8 +2256,8 @@
       <c r="K33" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="L33" s="96"/>
-      <c r="M33" s="98"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="91"/>
       <c r="N33" s="12" t="s">
         <v>98</v>
       </c>
@@ -2271,13 +2268,13 @@
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D34" s="4"/>
       <c r="E34" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F34" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G34" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H34" s="44"/>
       <c r="I34" s="40" t="s">
@@ -2405,12 +2402,12 @@
       <c r="J40" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="K40" s="96" t="s">
+      <c r="K40" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="97"/>
-      <c r="M40" s="97"/>
-      <c r="N40" s="98"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="91"/>
       <c r="O40" s="10" t="s">
         <v>1</v>
       </c>
@@ -2420,7 +2417,7 @@
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D41" s="4"/>
       <c r="E41" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -2447,12 +2444,12 @@
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="41"/>
-      <c r="K42" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L42" s="91"/>
-      <c r="M42" s="91"/>
-      <c r="N42" s="92"/>
+      <c r="K42" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" s="96"/>
+      <c r="M42" s="96"/>
+      <c r="N42" s="97"/>
       <c r="O42" s="41"/>
       <c r="P42" s="46"/>
       <c r="Q42" s="4"/>
@@ -2460,7 +2457,7 @@
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D43" s="4"/>
       <c r="E43" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
@@ -2469,12 +2466,12 @@
       <c r="J43" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L43" s="91"/>
-      <c r="M43" s="91"/>
-      <c r="N43" s="92"/>
+      <c r="K43" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L43" s="96"/>
+      <c r="M43" s="96"/>
+      <c r="N43" s="97"/>
       <c r="O43" s="41"/>
       <c r="P43" s="46"/>
       <c r="Q43" s="4"/>
@@ -2552,12 +2549,12 @@
       <c r="J46" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K46" s="93" t="s">
+      <c r="K46" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="94"/>
-      <c r="M46" s="94"/>
-      <c r="N46" s="95"/>
+      <c r="L46" s="99"/>
+      <c r="M46" s="99"/>
+      <c r="N46" s="100"/>
       <c r="O46" s="10"/>
       <c r="P46" s="32" t="s">
         <v>33</v>
@@ -2567,7 +2564,7 @@
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D47" s="4"/>
       <c r="E47" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="19"/>
@@ -2594,12 +2591,12 @@
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L48" s="91"/>
-      <c r="M48" s="91"/>
-      <c r="N48" s="92"/>
+      <c r="K48" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="97"/>
       <c r="O48" s="41"/>
       <c r="P48" s="46" t="s">
         <v>105</v>
@@ -2609,7 +2606,7 @@
     <row r="49" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D49" s="4"/>
       <c r="E49" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
@@ -2618,12 +2615,12 @@
       <c r="J49" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L49" s="91"/>
-      <c r="M49" s="91"/>
-      <c r="N49" s="92"/>
+      <c r="K49" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="96"/>
+      <c r="M49" s="96"/>
+      <c r="N49" s="97"/>
       <c r="O49" s="41"/>
       <c r="P49" s="46" t="s">
         <v>105</v>
@@ -2678,10 +2675,10 @@
       <c r="K52" s="9"/>
       <c r="L52" s="5"/>
       <c r="M52" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O52" s="4"/>
       <c r="R52" s="9"/>
@@ -2691,7 +2688,7 @@
     <row r="53" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D53" s="4"/>
       <c r="E53" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F53" s="36" t="s">
         <v>67</v>
@@ -2707,10 +2704,10 @@
       </c>
       <c r="L53" s="10"/>
       <c r="M53" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O53" s="4"/>
       <c r="Q53" s="2" t="s">
@@ -2725,7 +2722,7 @@
     <row r="54" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D54" s="4"/>
       <c r="E54" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F54" s="37" t="s">
         <v>68</v>
@@ -2734,17 +2731,17 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
       <c r="J54" s="14" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="K54" s="17" t="s">
         <v>25</v>
       </c>
       <c r="L54" s="13"/>
       <c r="M54" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O54" s="4"/>
       <c r="R54" s="12"/>
@@ -2792,7 +2789,7 @@
         <v>105</v>
       </c>
       <c r="N56" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O56" s="4"/>
       <c r="R56" s="41"/>
@@ -2868,10 +2865,10 @@
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N58" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q58" s="2" t="s">
         <v>11</v>
@@ -2883,7 +2880,7 @@
     <row r="59" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D59" s="4"/>
       <c r="E59" s="86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F59" s="36" t="s">
         <v>67</v>
@@ -2903,10 +2900,10 @@
         <v>17</v>
       </c>
       <c r="M59" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R59" s="21" t="s">
         <v>21</v>
@@ -2921,7 +2918,7 @@
     <row r="60" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D60" s="4"/>
       <c r="E60" s="87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F60" s="37" t="s">
         <v>68</v>
@@ -2934,7 +2931,7 @@
       </c>
       <c r="I60" s="13"/>
       <c r="J60" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K60" s="17" t="s">
         <v>66</v>
@@ -2943,10 +2940,10 @@
         <v>25</v>
       </c>
       <c r="M60" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N60" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R60" s="14" t="s">
         <v>22</v>
@@ -2982,11 +2979,11 @@
       <c r="N61" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="R61" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="S61" s="91"/>
-      <c r="T61" s="92"/>
+      <c r="R61" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="S61" s="96"/>
+      <c r="T61" s="97"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D62" s="4"/>
@@ -3010,13 +3007,13 @@
         <v>105</v>
       </c>
       <c r="N62" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="R62" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="S62" s="91"/>
-      <c r="T62" s="92"/>
+        <v>108</v>
+      </c>
+      <c r="R62" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="S62" s="96"/>
+      <c r="T62" s="97"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D63" s="4"/>
@@ -3043,7 +3040,7 @@
     <row r="64" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3203,7 +3200,7 @@
         <v>29</v>
       </c>
       <c r="J73" s="73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -3247,13 +3244,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E22:M22"/>
-    <mergeCell ref="E23:M23"/>
     <mergeCell ref="R61:T61"/>
     <mergeCell ref="R62:T62"/>
     <mergeCell ref="K46:N46"/>
@@ -3262,6 +3252,13 @@
     <mergeCell ref="K43:N43"/>
     <mergeCell ref="K48:N48"/>
     <mergeCell ref="K49:N49"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E22:M22"/>
+    <mergeCell ref="E23:M23"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E17 N16:P17 E22:E23 N22:P23 E29:Q30 E35:Q36 E42:P43 E48:P49 E55:N56 R55:T56 E61:N62 R61:R62">
     <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="~?">

</xml_diff>

<commit_message>
background processes on status line
</commit_message>
<xml_diff>
--- a/windowmanager/shortcuts.xlsx
+++ b/windowmanager/shortcuts.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruud.wijtvliet/.dotfiles/windowmanager/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B41EECA-A450-D447-B8DA-F5778A5EEA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16660" yWindow="700" windowWidth="13300" windowHeight="32400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16665" yWindow="705" windowWidth="13305" windowHeight="32400"/>
   </bookViews>
   <sheets>
     <sheet name="shortcuts" sheetId="1" r:id="rId1"/>
@@ -25,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruud Wijtvliet</author>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{B988E697-2D5A-AD45-80B6-3EB432B39195}">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{031F1851-94BB-B04D-B4A0-61F07FD025F6}">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{6DB6A60B-65B3-1141-8DED-B39904A2A8E3}">
+    <comment ref="F10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="161">
   <si>
     <t>ENTER</t>
   </si>
@@ -593,16 +587,40 @@
   </si>
   <si>
     <t>(= insert on right)</t>
+  </si>
+  <si>
+    <t>wezterm</t>
+  </si>
+  <si>
+    <t>other terminal</t>
+  </si>
+  <si>
+    <t>(backup)</t>
+  </si>
+  <si>
+    <t>force</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>monitors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1128,6 +1146,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,28 +1170,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1477,32 +1495,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.875" style="2"/>
     <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
     <col min="4" max="16" width="11.5" style="2" customWidth="1"/>
-    <col min="17" max="19" width="11.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.83203125" style="2"/>
+    <col min="17" max="19" width="11.875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" ht="15">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1510,7 +1528,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="15">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1518,7 +1536,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" ht="15">
       <c r="E5" s="48" t="s">
         <v>124</v>
       </c>
@@ -1556,7 +1574,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" ht="15">
       <c r="B6" s="78" t="s">
         <v>12</v>
       </c>
@@ -1575,15 +1593,19 @@
       <c r="I6" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>156</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="8"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21" ht="15">
       <c r="B7" s="78"/>
       <c r="E7" s="70" t="s">
         <v>121</v>
@@ -1600,15 +1622,19 @@
       <c r="I7" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="J7" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>159</v>
+      </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
       <c r="P7" s="81"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21" ht="15">
       <c r="B8" s="78"/>
       <c r="E8" s="71" t="s">
         <v>123</v>
@@ -1623,15 +1649,19 @@
         <v>142</v>
       </c>
       <c r="I8" s="74"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="J8" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>160</v>
+      </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="16"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" ht="15">
       <c r="B9" s="78"/>
       <c r="E9" s="18" t="s">
         <v>105</v>
@@ -1648,15 +1678,19 @@
       <c r="I9" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
+      <c r="J9" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="75" t="s">
+        <v>105</v>
+      </c>
       <c r="L9" s="75"/>
       <c r="M9" s="75"/>
       <c r="N9" s="75"/>
       <c r="O9" s="19"/>
       <c r="P9" s="20"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" ht="15">
       <c r="B10" s="78"/>
       <c r="E10" s="18" t="s">
         <v>105</v>
@@ -1673,29 +1707,33 @@
       <c r="I10" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="J10" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>108</v>
+      </c>
       <c r="L10" s="75"/>
       <c r="M10" s="75"/>
       <c r="N10" s="75"/>
       <c r="O10" s="19"/>
       <c r="P10" s="20"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" ht="15">
       <c r="B11" s="78"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" ht="15">
       <c r="B12" s="78"/>
       <c r="Q12" s="4"/>
       <c r="T12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" ht="15">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1722,21 +1760,21 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" ht="15">
       <c r="D14" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="99" t="s">
+      <c r="E14" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
       <c r="N14" s="88"/>
       <c r="O14" s="12" t="s">
         <v>21</v>
@@ -1752,7 +1790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" ht="15">
       <c r="D15" s="37" t="s">
         <v>137</v>
       </c>
@@ -1780,22 +1818,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" ht="15">
       <c r="C16" s="2" t="s">
         <v>109</v>
       </c>
       <c r="D16" s="45"/>
-      <c r="E16" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="91"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="91"/>
+      <c r="E16" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="96"/>
+      <c r="M16" s="96"/>
       <c r="N16" s="89"/>
       <c r="O16" s="13" t="s">
         <v>105</v>
@@ -1811,22 +1849,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:21" ht="15">
       <c r="C17" s="2" t="s">
         <v>110</v>
       </c>
       <c r="D17" s="45"/>
-      <c r="E17" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
+      <c r="E17" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
       <c r="N17" s="89"/>
       <c r="O17" s="13" t="s">
         <v>108</v>
@@ -1842,7 +1880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" ht="15">
       <c r="D18" s="60" t="s">
         <v>10</v>
       </c>
@@ -1887,7 +1925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:21" ht="15">
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1916,21 +1954,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:21" ht="15">
       <c r="D20" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="96" t="s">
+      <c r="E20" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="97"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="97"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
       <c r="N20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +1986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:21" ht="15">
       <c r="D21" s="37" t="s">
         <v>137</v>
       </c>
@@ -1978,21 +2016,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:21" ht="15">
       <c r="D22" s="45"/>
-      <c r="E22" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
+      <c r="E22" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
       <c r="N22" s="41" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O22" s="13" t="s">
         <v>105</v>
@@ -2002,19 +2040,19 @@
       </c>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" ht="15">
       <c r="D23" s="45"/>
-      <c r="E23" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
+      <c r="E23" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
       <c r="N23" s="41" t="s">
         <v>105</v>
       </c>
@@ -2026,7 +2064,7 @@
       </c>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:21" ht="15">
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2042,7 +2080,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:21" ht="15">
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2071,7 +2109,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="25"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:21" ht="15">
       <c r="D27" s="4"/>
       <c r="E27" s="86" t="s">
         <v>146</v>
@@ -2099,7 +2137,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="27"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:21" ht="15">
       <c r="D28" s="4"/>
       <c r="E28" s="87" t="s">
         <v>147</v>
@@ -2127,7 +2165,7 @@
       <c r="P28" s="13"/>
       <c r="Q28" s="20"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:21" ht="15">
       <c r="D29" s="4"/>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -2147,7 +2185,7 @@
       <c r="P29" s="41"/>
       <c r="Q29" s="41"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:21" ht="15">
       <c r="D30" s="4"/>
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
@@ -2167,7 +2205,7 @@
       <c r="P30" s="41"/>
       <c r="Q30" s="41"/>
     </row>
-    <row r="31" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:21" ht="15.95">
       <c r="E31" s="51" t="s">
         <v>2</v>
       </c>
@@ -2208,7 +2246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:21" ht="15">
       <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
@@ -2235,7 +2273,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="25"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" ht="15">
       <c r="D33" s="4"/>
       <c r="E33" s="86" t="s">
         <v>146</v>
@@ -2256,8 +2294,8 @@
       <c r="K33" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="L33" s="96"/>
-      <c r="M33" s="98"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="91"/>
       <c r="N33" s="12" t="s">
         <v>98</v>
       </c>
@@ -2265,7 +2303,7 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="27"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" ht="15">
       <c r="D34" s="4"/>
       <c r="E34" s="87" t="s">
         <v>147</v>
@@ -2293,7 +2331,7 @@
       <c r="P34" s="13"/>
       <c r="Q34" s="20"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" ht="15">
       <c r="D35" s="4"/>
       <c r="E35" s="41"/>
       <c r="F35" s="41"/>
@@ -2315,7 +2353,7 @@
       <c r="P35" s="41"/>
       <c r="Q35" s="41"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" ht="15">
       <c r="D36" s="4"/>
       <c r="E36" s="41"/>
       <c r="F36" s="41"/>
@@ -2337,7 +2375,7 @@
       <c r="P36" s="41"/>
       <c r="Q36" s="41"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" ht="15">
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2353,7 +2391,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" ht="15">
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2369,7 +2407,7 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17" ht="15">
       <c r="B39" s="2" t="s">
         <v>12</v>
       </c>
@@ -2390,7 +2428,7 @@
       <c r="P39" s="28"/>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17" ht="15">
       <c r="D40" s="4"/>
       <c r="E40" s="21" t="s">
         <v>98</v>
@@ -2402,19 +2440,21 @@
       <c r="J40" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="K40" s="96" t="s">
+      <c r="K40" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="97"/>
-      <c r="M40" s="97"/>
-      <c r="N40" s="98"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="91"/>
       <c r="O40" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="P40" s="29"/>
+      <c r="P40" s="29" t="s">
+        <v>154</v>
+      </c>
       <c r="Q40" s="4"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17" ht="15">
       <c r="D41" s="4"/>
       <c r="E41" s="14" t="s">
         <v>106</v>
@@ -2431,10 +2471,12 @@
       <c r="M41" s="15"/>
       <c r="N41" s="16"/>
       <c r="O41" s="13"/>
-      <c r="P41" s="30"/>
+      <c r="P41" s="30" t="s">
+        <v>155</v>
+      </c>
       <c r="Q41" s="4"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" ht="15">
       <c r="D42" s="4"/>
       <c r="E42" s="41" t="s">
         <v>105</v>
@@ -2444,17 +2486,17 @@
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="41"/>
-      <c r="K42" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L42" s="91"/>
-      <c r="M42" s="91"/>
-      <c r="N42" s="92"/>
+      <c r="K42" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" s="96"/>
+      <c r="M42" s="96"/>
+      <c r="N42" s="97"/>
       <c r="O42" s="41"/>
       <c r="P42" s="46"/>
       <c r="Q42" s="4"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" ht="15">
       <c r="D43" s="4"/>
       <c r="E43" s="41" t="s">
         <v>108</v>
@@ -2466,17 +2508,17 @@
       <c r="J43" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L43" s="91"/>
-      <c r="M43" s="91"/>
-      <c r="N43" s="92"/>
+      <c r="K43" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L43" s="96"/>
+      <c r="M43" s="96"/>
+      <c r="N43" s="97"/>
       <c r="O43" s="41"/>
       <c r="P43" s="46"/>
       <c r="Q43" s="4"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" ht="15">
       <c r="D44" s="4"/>
       <c r="E44" s="51" t="s">
         <v>47</v>
@@ -2516,7 +2558,7 @@
       </c>
       <c r="Q44" s="4"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" ht="15">
       <c r="B45" s="2" t="s">
         <v>11</v>
       </c>
@@ -2537,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17" ht="15">
       <c r="D46" s="4"/>
       <c r="E46" s="21" t="s">
         <v>98</v>
@@ -2549,19 +2591,19 @@
       <c r="J46" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K46" s="93" t="s">
+      <c r="K46" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="94"/>
-      <c r="M46" s="94"/>
-      <c r="N46" s="95"/>
+      <c r="L46" s="99"/>
+      <c r="M46" s="99"/>
+      <c r="N46" s="100"/>
       <c r="O46" s="10"/>
       <c r="P46" s="32" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="Q46" s="4"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17" ht="15">
       <c r="D47" s="4"/>
       <c r="E47" s="14" t="s">
         <v>107</v>
@@ -2581,7 +2623,7 @@
       <c r="P47" s="34"/>
       <c r="Q47" s="4"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17" ht="15">
       <c r="D48" s="4"/>
       <c r="E48" s="41" t="s">
         <v>105</v>
@@ -2591,19 +2633,19 @@
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
       <c r="J48" s="47"/>
-      <c r="K48" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L48" s="91"/>
-      <c r="M48" s="91"/>
-      <c r="N48" s="92"/>
+      <c r="K48" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="97"/>
       <c r="O48" s="41"/>
       <c r="P48" s="46" t="s">
         <v>105</v>
       </c>
       <c r="Q48" s="4"/>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:20" ht="15">
       <c r="D49" s="4"/>
       <c r="E49" s="41" t="s">
         <v>108</v>
@@ -2615,19 +2657,19 @@
       <c r="J49" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="L49" s="91"/>
-      <c r="M49" s="91"/>
-      <c r="N49" s="92"/>
+      <c r="K49" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="96"/>
+      <c r="M49" s="96"/>
+      <c r="N49" s="97"/>
       <c r="O49" s="41"/>
       <c r="P49" s="46" t="s">
         <v>105</v>
       </c>
       <c r="Q49" s="4"/>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:20" ht="15">
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -2641,7 +2683,7 @@
       <c r="N50" s="4"/>
       <c r="P50" s="4"/>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:20" ht="15">
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -2655,7 +2697,7 @@
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:20" ht="15">
       <c r="B52" s="2" t="s">
         <v>12</v>
       </c>
@@ -2685,7 +2727,7 @@
       <c r="S52" s="9"/>
       <c r="T52" s="9"/>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:20" ht="15">
       <c r="D53" s="4"/>
       <c r="E53" s="86" t="s">
         <v>146</v>
@@ -2719,7 +2761,7 @@
       </c>
       <c r="T53" s="12"/>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:20" ht="15">
       <c r="D54" s="4"/>
       <c r="E54" s="87" t="s">
         <v>147</v>
@@ -2750,7 +2792,7 @@
       </c>
       <c r="T54" s="12"/>
     </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:20" ht="15">
       <c r="D55" s="4"/>
       <c r="E55" s="41"/>
       <c r="F55" s="41"/>
@@ -2775,7 +2817,7 @@
       </c>
       <c r="T55" s="41"/>
     </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:20" ht="15">
       <c r="D56" s="4"/>
       <c r="E56" s="41"/>
       <c r="F56" s="41"/>
@@ -2798,7 +2840,7 @@
       </c>
       <c r="T56" s="41"/>
     </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:20" ht="15">
       <c r="D57" s="4"/>
       <c r="E57" s="48" t="s">
         <v>9</v>
@@ -2841,7 +2883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:20" ht="15">
       <c r="B58" s="2" t="s">
         <v>11</v>
       </c>
@@ -2877,7 +2919,7 @@
       <c r="S58" s="7"/>
       <c r="T58" s="8"/>
     </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:20" ht="15">
       <c r="D59" s="4"/>
       <c r="E59" s="86" t="s">
         <v>146</v>
@@ -2915,7 +2957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:20" ht="15">
       <c r="D60" s="4"/>
       <c r="E60" s="87" t="s">
         <v>147</v>
@@ -2955,7 +2997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:20" ht="15">
       <c r="D61" s="4"/>
       <c r="E61" s="41"/>
       <c r="F61" s="41"/>
@@ -2979,13 +3021,13 @@
       <c r="N61" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="R61" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="S61" s="91"/>
-      <c r="T61" s="92"/>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="R61" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="S61" s="96"/>
+      <c r="T61" s="97"/>
+    </row>
+    <row r="62" spans="2:20" ht="15">
       <c r="D62" s="4"/>
       <c r="E62" s="41"/>
       <c r="F62" s="41"/>
@@ -3009,13 +3051,13 @@
       <c r="N62" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="R62" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="S62" s="91"/>
-      <c r="T62" s="92"/>
-    </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="R62" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="S62" s="96"/>
+      <c r="T62" s="97"/>
+    </row>
+    <row r="63" spans="2:20" ht="15">
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3037,7 +3079,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:20" ht="15">
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
         <v>139</v>
@@ -3056,7 +3098,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:18" ht="15">
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -3071,7 +3113,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:18" ht="15">
       <c r="B66" s="2" t="s">
         <v>12</v>
       </c>
@@ -3093,7 +3135,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:18" ht="15">
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -3109,7 +3151,7 @@
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:18" ht="15">
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -3125,7 +3167,7 @@
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:18" ht="15">
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3139,7 +3181,7 @@
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:18" ht="15">
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -3153,7 +3195,7 @@
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:18" ht="15">
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -3171,7 +3213,7 @@
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:18" ht="15">
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
@@ -3190,7 +3232,7 @@
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
     </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:18" ht="15">
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -3208,7 +3250,7 @@
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:18" ht="15">
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3224,7 +3266,7 @@
       <c r="N74" s="4"/>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:18" ht="15">
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -3238,19 +3280,12 @@
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:18" ht="15">
       <c r="I76" s="45"/>
       <c r="J76" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="E14:M14"/>
-    <mergeCell ref="E16:M16"/>
-    <mergeCell ref="E17:M17"/>
-    <mergeCell ref="E22:M22"/>
-    <mergeCell ref="E23:M23"/>
     <mergeCell ref="R61:T61"/>
     <mergeCell ref="R62:T62"/>
     <mergeCell ref="K46:N46"/>
@@ -3259,6 +3294,13 @@
     <mergeCell ref="K43:N43"/>
     <mergeCell ref="K48:N48"/>
     <mergeCell ref="K49:N49"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="E14:M14"/>
+    <mergeCell ref="E16:M16"/>
+    <mergeCell ref="E17:M17"/>
+    <mergeCell ref="E22:M22"/>
+    <mergeCell ref="E23:M23"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E17 N16:P17 E22:E23 N22:P23 E29:Q30 E35:Q36 E42:P43 E48:P49 E55:N56 R55:T56 E61:N62 R61:R62">
     <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="~?">

</xml_diff>

<commit_message>
window management on windows
</commit_message>
<xml_diff>
--- a/windowmanager/shortcuts.xlsx
+++ b/windowmanager/shortcuts.xlsx
@@ -22,6 +22,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruud Wijtvliet</author>
+    <author>r</author>
   </authors>
   <commentList>
     <comment ref="E9" authorId="0">
@@ -54,6 +55,54 @@
             <family val="2"/>
           </rPr>
           <t>works on linux/i3?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not needed; automatic</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not needed; automatic</t>
         </r>
       </text>
     </comment>
@@ -123,12 +172,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="J11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not needed; automatic</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not needed; automatic</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J70" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+*force floating</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M70" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>r:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+*toggles between horizontal and vertical</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="156">
   <si>
     <t>ENTER</t>
   </si>
@@ -448,33 +593,15 @@
     <t>yes</t>
   </si>
   <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>child</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>works on linux / i3?</t>
-  </si>
-  <si>
     <t>works on macos/yabai?</t>
   </si>
   <si>
     <t>floating/tiled</t>
   </si>
   <si>
-    <t>to tiling</t>
-  </si>
-  <si>
-    <t>set/toggle</t>
-  </si>
-  <si>
-    <t>layout</t>
-  </si>
-  <si>
     <t>Open app</t>
   </si>
   <si>
@@ -487,12 +614,6 @@
     <t>horizontal</t>
   </si>
   <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>to stacking</t>
-  </si>
-  <si>
     <t>layout to</t>
   </si>
   <si>
@@ -613,7 +734,13 @@
     <t>monitors</t>
   </si>
   <si>
-    <t>works on windows</t>
+    <t>?</t>
+  </si>
+  <si>
+    <t>works on linux/i3?</t>
+  </si>
+  <si>
+    <t>works on windows/glazeWM?</t>
   </si>
 </sst>
 </file>
@@ -623,7 +750,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +799,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -894,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1158,6 +1298,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1176,19 +1334,34 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1196,7 +1369,91 @@
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1549,7 +1806,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1559,15 +1816,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="2"/>
     <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="2" customWidth="1"/>
     <col min="4" max="16" width="11.5" style="2" customWidth="1"/>
     <col min="17" max="19" width="11.875" style="2" customWidth="1"/>
     <col min="20" max="20" width="10.875" style="2" customWidth="1"/>
@@ -1592,40 +1849,40 @@
     </row>
     <row r="5" spans="2:21" ht="15">
       <c r="E5" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="N5" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="O5" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="76" t="s">
+      <c r="P5" s="50" t="s">
         <v>127</v>
-      </c>
-      <c r="I5" s="77" t="s">
-        <v>128</v>
-      </c>
-      <c r="J5" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="L5" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="M5" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="N5" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="O5" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="P5" s="50" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="15">
@@ -1639,19 +1896,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I6" s="72" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1662,25 +1919,25 @@
     <row r="7" spans="2:21" ht="15">
       <c r="B7" s="78"/>
       <c r="E7" s="70" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H7" s="81" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="73" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
@@ -1691,23 +1948,23 @@
     <row r="8" spans="2:21" ht="15">
       <c r="B8" s="78"/>
       <c r="E8" s="71" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F8" s="84" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I8" s="74"/>
       <c r="J8" s="15" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1732,10 +1989,10 @@
       <c r="I9" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="K9" s="75" t="s">
+      <c r="J9" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="93" t="s">
         <v>105</v>
       </c>
       <c r="L9" s="75"/>
@@ -1748,11 +2005,19 @@
       <c r="B10" s="78"/>
       <c r="E10" s="18"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="92"/>
+      <c r="G10" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="92" t="s">
+        <v>153</v>
+      </c>
       <c r="I10" s="41"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="J10" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" s="93" t="s">
+        <v>106</v>
+      </c>
       <c r="L10" s="75"/>
       <c r="M10" s="75"/>
       <c r="N10" s="75"/>
@@ -1776,11 +2041,11 @@
       <c r="I11" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="K11" s="75" t="s">
-        <v>108</v>
+      <c r="J11" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="93" t="s">
+        <v>106</v>
       </c>
       <c r="L11" s="75"/>
       <c r="M11" s="75"/>
@@ -1831,19 +2096,19 @@
     </row>
     <row r="15" spans="2:21">
       <c r="D15" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="102" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="103"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="103"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
       <c r="N15" s="88"/>
       <c r="O15" s="12" t="s">
         <v>21</v>
@@ -1861,7 +2126,7 @@
     </row>
     <row r="16" spans="2:21">
       <c r="D16" s="37" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
@@ -1889,20 +2154,20 @@
     </row>
     <row r="17" spans="2:21">
       <c r="C17" s="2" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="D17" s="45"/>
-      <c r="E17" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
+      <c r="E17" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="100"/>
+      <c r="M17" s="100"/>
       <c r="N17" s="89"/>
       <c r="O17" s="13" t="s">
         <v>105</v>
@@ -1920,45 +2185,51 @@
     </row>
     <row r="18" spans="2:21">
       <c r="C18" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D18" s="45"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="91"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="91"/>
-      <c r="M18" s="91"/>
+      <c r="E18" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
       <c r="N18" s="89"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
+      <c r="O18" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="P18" s="13" t="s">
+        <v>153</v>
+      </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="2:21">
       <c r="C19" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D19" s="45"/>
-      <c r="E19" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="95"/>
+      <c r="E19" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="101"/>
       <c r="N19" s="89"/>
       <c r="O19" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="T19" s="2">
@@ -2030,7 +2301,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="9" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="O21" s="7"/>
       <c r="P21" s="9"/>
@@ -2044,19 +2315,19 @@
     </row>
     <row r="22" spans="2:21">
       <c r="D22" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="99" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="100"/>
-      <c r="G22" s="100"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="100"/>
-      <c r="K22" s="100"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="100"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
       <c r="N22" s="12" t="s">
         <v>25</v>
       </c>
@@ -2076,7 +2347,7 @@
     </row>
     <row r="23" spans="2:21">
       <c r="D23" s="37" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
@@ -2088,7 +2359,7 @@
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
       <c r="N23" s="17" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="O23" s="15" t="s">
         <v>22</v>
@@ -2106,19 +2377,19 @@
     </row>
     <row r="24" spans="2:21">
       <c r="D24" s="45"/>
-      <c r="E24" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="M24" s="94"/>
+      <c r="E24" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
       <c r="N24" s="41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O24" s="13" t="s">
         <v>105</v>
@@ -2130,41 +2401,49 @@
     </row>
     <row r="25" spans="2:21">
       <c r="D25" s="45"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="94"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="94"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
+      <c r="E25" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="O25" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="P25" s="13" t="s">
+        <v>153</v>
+      </c>
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="2:21">
       <c r="D26" s="45"/>
-      <c r="E26" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="94"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="94"/>
-      <c r="I26" s="94"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="94"/>
-      <c r="L26" s="94"/>
-      <c r="M26" s="94"/>
+      <c r="E26" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
       <c r="N26" s="41" t="s">
         <v>105</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P26" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q26" s="4"/>
     </row>
@@ -2216,13 +2495,13 @@
     <row r="30" spans="2:21">
       <c r="D30" s="4"/>
       <c r="E30" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F30" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G30" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="43" t="s">
@@ -2244,13 +2523,13 @@
     <row r="31" spans="2:21">
       <c r="D31" s="4"/>
       <c r="E31" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F31" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G31" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="44" t="s">
@@ -2297,10 +2576,14 @@
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
       <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
+      <c r="K33" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
+      <c r="N33" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="O33" s="41"/>
       <c r="P33" s="41"/>
       <c r="Q33" s="41"/>
@@ -2381,7 +2664,7 @@
         <v>28</v>
       </c>
       <c r="H36" s="42" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I36" s="38"/>
       <c r="J36" s="6"/>
@@ -2396,16 +2679,16 @@
     <row r="37" spans="2:17">
       <c r="D37" s="4"/>
       <c r="E37" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F37" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G37" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="H37" s="43" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>93</v>
@@ -2414,8 +2697,8 @@
       <c r="K37" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="L37" s="99"/>
-      <c r="M37" s="101"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="95"/>
       <c r="N37" s="12" t="s">
         <v>98</v>
       </c>
@@ -2426,13 +2709,13 @@
     <row r="38" spans="2:17">
       <c r="D38" s="4"/>
       <c r="E38" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F38" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G38" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="40" t="s">
@@ -2478,13 +2761,19 @@
       <c r="E40" s="41"/>
       <c r="F40" s="41"/>
       <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
+      <c r="H40" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="I40" s="46"/>
       <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
+      <c r="K40" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="L40" s="41"/>
       <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
+      <c r="N40" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="O40" s="41"/>
       <c r="P40" s="41"/>
       <c r="Q40" s="41"/>
@@ -2494,7 +2783,9 @@
       <c r="E41" s="41"/>
       <c r="F41" s="41"/>
       <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
+      <c r="H41" s="41" t="s">
+        <v>106</v>
+      </c>
       <c r="I41" s="46" t="s">
         <v>105</v>
       </c>
@@ -2548,7 +2839,7 @@
         <v>12</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="109"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
@@ -2566,9 +2857,7 @@
     </row>
     <row r="45" spans="2:17">
       <c r="D45" s="4"/>
-      <c r="E45" s="21" t="s">
-        <v>98</v>
-      </c>
+      <c r="E45" s="110"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -2576,25 +2865,23 @@
       <c r="J45" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="K45" s="99" t="s">
+      <c r="K45" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="L45" s="100"/>
-      <c r="M45" s="100"/>
-      <c r="N45" s="101"/>
+      <c r="L45" s="96"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="95"/>
       <c r="O45" s="10" t="s">
         <v>1</v>
       </c>
       <c r="P45" s="29" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="Q45" s="4"/>
     </row>
     <row r="46" spans="2:17">
       <c r="D46" s="4"/>
-      <c r="E46" s="14" t="s">
-        <v>106</v>
-      </c>
+      <c r="E46" s="111"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="H46" s="19"/>
@@ -2608,26 +2895,26 @@
       <c r="N46" s="16"/>
       <c r="O46" s="13"/>
       <c r="P46" s="30" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="Q46" s="4"/>
     </row>
     <row r="47" spans="2:17">
       <c r="D47" s="4"/>
-      <c r="E47" s="41" t="s">
-        <v>105</v>
-      </c>
+      <c r="E47" s="41"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
       <c r="H47" s="41"/>
       <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="L47" s="94"/>
-      <c r="M47" s="94"/>
-      <c r="N47" s="95"/>
+      <c r="J47" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="L47" s="100"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="101"/>
       <c r="O47" s="41"/>
       <c r="P47" s="46"/>
       <c r="Q47" s="4"/>
@@ -2639,20 +2926,22 @@
       <c r="G48" s="41"/>
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="91"/>
-      <c r="M48" s="91"/>
-      <c r="N48" s="92"/>
+      <c r="J48" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="L48" s="100"/>
+      <c r="M48" s="100"/>
+      <c r="N48" s="101"/>
       <c r="O48" s="41"/>
       <c r="P48" s="46"/>
       <c r="Q48" s="4"/>
     </row>
     <row r="49" spans="2:20">
       <c r="D49" s="4"/>
-      <c r="E49" s="41" t="s">
-        <v>108</v>
-      </c>
+      <c r="E49" s="41"/>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
       <c r="H49" s="41"/>
@@ -2660,12 +2949,12 @@
       <c r="J49" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="L49" s="94"/>
-      <c r="M49" s="94"/>
-      <c r="N49" s="95"/>
+      <c r="K49" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="100"/>
+      <c r="M49" s="100"/>
+      <c r="N49" s="101"/>
       <c r="O49" s="41"/>
       <c r="P49" s="46"/>
       <c r="Q49" s="4"/>
@@ -2715,8 +3004,8 @@
         <v>11</v>
       </c>
       <c r="D51" s="4"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="112"/>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
       <c r="I51" s="25"/>
@@ -2733,34 +3022,30 @@
     </row>
     <row r="52" spans="2:20">
       <c r="D52" s="4"/>
-      <c r="E52" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F52" s="22"/>
+      <c r="E52" s="110"/>
+      <c r="F52" s="113"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="27"/>
       <c r="J52" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K52" s="96" t="s">
+      <c r="K52" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="L52" s="97"/>
-      <c r="M52" s="97"/>
-      <c r="N52" s="98"/>
+      <c r="L52" s="103"/>
+      <c r="M52" s="103"/>
+      <c r="N52" s="104"/>
       <c r="O52" s="10"/>
       <c r="P52" s="32" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="Q52" s="4"/>
     </row>
     <row r="53" spans="2:20">
       <c r="D53" s="4"/>
-      <c r="E53" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F53" s="15"/>
+      <c r="E53" s="111"/>
+      <c r="F53" s="114"/>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
       <c r="I53" s="20"/>
@@ -2777,20 +3062,20 @@
     </row>
     <row r="54" spans="2:20">
       <c r="D54" s="4"/>
-      <c r="E54" s="41" t="s">
-        <v>105</v>
-      </c>
+      <c r="E54" s="41"/>
       <c r="F54" s="41"/>
       <c r="G54" s="41"/>
       <c r="H54" s="41"/>
       <c r="I54" s="41"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="L54" s="94"/>
-      <c r="M54" s="94"/>
-      <c r="N54" s="95"/>
+      <c r="J54" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="K54" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="L54" s="100"/>
+      <c r="M54" s="100"/>
+      <c r="N54" s="101"/>
       <c r="O54" s="41"/>
       <c r="P54" s="46" t="s">
         <v>105</v>
@@ -2804,20 +3089,24 @@
       <c r="G55" s="41"/>
       <c r="H55" s="41"/>
       <c r="I55" s="41"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="90"/>
-      <c r="L55" s="91"/>
-      <c r="M55" s="91"/>
-      <c r="N55" s="92"/>
+      <c r="J55" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="K55" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="L55" s="100"/>
+      <c r="M55" s="100"/>
+      <c r="N55" s="101"/>
       <c r="O55" s="41"/>
-      <c r="P55" s="46"/>
+      <c r="P55" s="46" t="s">
+        <v>153</v>
+      </c>
       <c r="Q55" s="4"/>
     </row>
     <row r="56" spans="2:20">
       <c r="D56" s="4"/>
-      <c r="E56" s="41" t="s">
-        <v>108</v>
-      </c>
+      <c r="E56" s="41"/>
       <c r="F56" s="41"/>
       <c r="G56" s="41"/>
       <c r="H56" s="41"/>
@@ -2825,12 +3114,12 @@
       <c r="J56" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="K56" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="L56" s="94"/>
-      <c r="M56" s="94"/>
-      <c r="N56" s="95"/>
+      <c r="K56" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="L56" s="100"/>
+      <c r="M56" s="100"/>
+      <c r="N56" s="101"/>
       <c r="O56" s="41"/>
       <c r="P56" s="46" t="s">
         <v>105</v>
@@ -2885,11 +3174,9 @@
       <c r="K59" s="9"/>
       <c r="L59" s="5"/>
       <c r="M59" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="N59" s="9" t="s">
-        <v>119</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="N59" s="106"/>
       <c r="O59" s="4"/>
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
@@ -2898,7 +3185,7 @@
     <row r="60" spans="2:20">
       <c r="D60" s="4"/>
       <c r="E60" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F60" s="36" t="s">
         <v>67</v>
@@ -2914,11 +3201,9 @@
       </c>
       <c r="L60" s="10"/>
       <c r="M60" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="N60" s="12" t="s">
-        <v>114</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N60" s="107"/>
       <c r="O60" s="4"/>
       <c r="Q60" s="2" t="s">
         <v>11</v>
@@ -2932,7 +3217,7 @@
     <row r="61" spans="2:20">
       <c r="D61" s="4"/>
       <c r="E61" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F61" s="37" t="s">
         <v>68</v>
@@ -2941,18 +3226,16 @@
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
       <c r="J61" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K61" s="17" t="s">
         <v>25</v>
       </c>
       <c r="L61" s="13"/>
       <c r="M61" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="N61" s="17" t="s">
-        <v>120</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="N61" s="108"/>
       <c r="O61" s="4"/>
       <c r="R61" s="12"/>
       <c r="S61" s="12" t="s">
@@ -2975,9 +3258,7 @@
       <c r="M62" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="N62" s="41" t="s">
-        <v>105</v>
-      </c>
+      <c r="N62" s="41"/>
       <c r="O62" s="4"/>
       <c r="R62" s="41"/>
       <c r="S62" s="41" t="s">
@@ -2992,10 +3273,16 @@
       <c r="G63" s="41"/>
       <c r="H63" s="41"/>
       <c r="I63" s="41"/>
-      <c r="J63" s="41"/>
-      <c r="K63" s="41"/>
+      <c r="J63" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="K63" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="L63" s="41"/>
-      <c r="M63" s="41"/>
+      <c r="M63" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="N63" s="41"/>
       <c r="O63" s="4"/>
       <c r="R63" s="41"/>
@@ -3015,9 +3302,7 @@
       <c r="M64" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="N64" s="41" t="s">
-        <v>108</v>
-      </c>
+      <c r="N64" s="41"/>
       <c r="O64" s="4"/>
       <c r="R64" s="41"/>
       <c r="S64" s="41" t="s">
@@ -3092,11 +3377,9 @@
       </c>
       <c r="L66" s="9"/>
       <c r="M66" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="N66" s="9" t="s">
-        <v>113</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="N66" s="106"/>
       <c r="Q66" s="2" t="s">
         <v>11</v>
       </c>
@@ -3107,7 +3390,7 @@
     <row r="67" spans="2:20">
       <c r="D67" s="4"/>
       <c r="E67" s="86" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F67" s="36" t="s">
         <v>67</v>
@@ -3127,11 +3410,9 @@
         <v>17</v>
       </c>
       <c r="M67" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="N67" s="12" t="s">
-        <v>114</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="N67" s="107"/>
       <c r="R67" s="21" t="s">
         <v>21</v>
       </c>
@@ -3145,7 +3426,7 @@
     <row r="68" spans="2:20">
       <c r="D68" s="4"/>
       <c r="E68" s="87" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F68" s="37" t="s">
         <v>68</v>
@@ -3158,7 +3439,7 @@
       </c>
       <c r="I68" s="13"/>
       <c r="J68" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K68" s="17" t="s">
         <v>66</v>
@@ -3167,11 +3448,9 @@
         <v>25</v>
       </c>
       <c r="M68" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>112</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="N68" s="108"/>
       <c r="R68" s="14" t="s">
         <v>22</v>
       </c>
@@ -3203,26 +3482,34 @@
       <c r="M69" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="N69" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="R69" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="S69" s="94"/>
-      <c r="T69" s="95"/>
+      <c r="N69" s="41"/>
+      <c r="R69" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="S69" s="100"/>
+      <c r="T69" s="101"/>
     </row>
     <row r="70" spans="2:20">
       <c r="D70" s="4"/>
       <c r="E70" s="41"/>
       <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
+      <c r="G70" s="41" t="s">
+        <v>106</v>
+      </c>
       <c r="H70" s="41"/>
       <c r="I70" s="41"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="41"/>
-      <c r="L70" s="41"/>
-      <c r="M70" s="41"/>
+      <c r="J70" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="K70" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="L70" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="M70" s="41" t="s">
+        <v>153</v>
+      </c>
       <c r="N70" s="41"/>
       <c r="R70" s="90"/>
       <c r="S70" s="91"/>
@@ -3249,14 +3536,12 @@
       <c r="M71" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="N71" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="R71" s="93" t="s">
-        <v>105</v>
-      </c>
-      <c r="S71" s="94"/>
-      <c r="T71" s="95"/>
+      <c r="N71" s="41"/>
+      <c r="R71" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="S71" s="100"/>
+      <c r="T71" s="101"/>
     </row>
     <row r="72" spans="2:20" ht="15">
       <c r="D72" s="4"/>
@@ -3283,7 +3568,7 @@
     <row r="73" spans="2:20">
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -3457,7 +3742,7 @@
         <v>29</v>
       </c>
       <c r="J83" s="73" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
@@ -3514,7 +3799,17 @@
       <c r="J87" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
+    <mergeCell ref="R69:T69"/>
+    <mergeCell ref="R71:T71"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K48:N48"/>
     <mergeCell ref="L37:M37"/>
     <mergeCell ref="E22:M22"/>
     <mergeCell ref="E15:M15"/>
@@ -3523,46 +3818,50 @@
     <mergeCell ref="E26:M26"/>
     <mergeCell ref="E19:M19"/>
     <mergeCell ref="E25:M25"/>
-    <mergeCell ref="R69:T69"/>
-    <mergeCell ref="R71:T71"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="E18:M18"/>
   </mergeCells>
-  <conditionalFormatting sqref="E17:E19 N17:P19 E24 N24:P24 E32:Q34 E39:Q41 E47:P49 E54:P56 E62:N64 R62:T64 E69:N71 R69:R71 N26:P26 E26">
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="~?">
+  <conditionalFormatting sqref="E17 N17:P19 E24 N24:P24 E32:Q34 E39:Q41 E62:N64 R62:T64 E69:N71 R69:R71 N26:P26 E26 E19 E54:P56 E47:P49">
+    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="~?">
       <formula>NOT(ISERROR(SEARCH("~?",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="14" stopIfTrue="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="22" priority="17" stopIfTrue="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:P12">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="~?">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="~?">
       <formula>NOT(ISERROR(SEARCH("~?",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" stopIfTrue="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="19" priority="8" stopIfTrue="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:P25 E25">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="~?">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="~?">
       <formula>NOT(ISERROR(SEARCH("~?",E25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" stopIfTrue="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="16" priority="5" stopIfTrue="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",E25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",E25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="~?">
+      <formula>NOT(ISERROR(SEARCH("~?",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>